<commit_message>
Google mobility and MYS data update.
</commit_message>
<xml_diff>
--- a/data/inputs/covid_mys/COVID_MYS_CASE.xlsx
+++ b/data/inputs/covid_mys/COVID_MYS_CASE.xlsx
@@ -2156,7 +2156,7 @@
         <v>1780.0</v>
       </c>
       <c r="E77" s="10">
-        <f t="shared" ref="E77:E220" si="3">D77-F77</f>
+        <f t="shared" ref="E77:E227" si="3">D77-F77</f>
         <v>1753</v>
       </c>
       <c r="F77" s="19">
@@ -6062,33 +6062,194 @@
       <c r="A220" s="8">
         <v>44097.0</v>
       </c>
-      <c r="B220" s="21">
+      <c r="B220" s="20">
         <v>147.0</v>
       </c>
-      <c r="C220" s="21">
+      <c r="C220" s="20">
         <v>4.0</v>
       </c>
-      <c r="D220" s="21">
+      <c r="D220" s="20">
         <v>770.0</v>
       </c>
       <c r="E220" s="10">
         <f t="shared" si="3"/>
         <v>762</v>
       </c>
-      <c r="F220" s="21">
+      <c r="F220" s="20">
         <v>8.0</v>
       </c>
-      <c r="G220" s="21">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
+      <c r="G220" s="20">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="221" ht="15.75" customHeight="1">
+      <c r="A221" s="8">
+        <v>44098.0</v>
+      </c>
+      <c r="B221" s="20">
+        <v>71.0</v>
+      </c>
+      <c r="C221" s="20">
+        <v>2.0</v>
+      </c>
+      <c r="D221" s="20">
+        <v>777.0</v>
+      </c>
+      <c r="E221" s="10">
+        <f t="shared" si="3"/>
+        <v>771</v>
+      </c>
+      <c r="F221" s="20">
+        <v>6.0</v>
+      </c>
+      <c r="G221" s="20">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="222" ht="15.75" customHeight="1">
+      <c r="A222" s="8">
+        <v>44099.0</v>
+      </c>
+      <c r="B222" s="20">
+        <v>111.0</v>
+      </c>
+      <c r="C222" s="20">
+        <v>4.0</v>
+      </c>
+      <c r="D222" s="20">
+        <v>858.0</v>
+      </c>
+      <c r="E222" s="10">
+        <f t="shared" si="3"/>
+        <v>854</v>
+      </c>
+      <c r="F222" s="20">
+        <v>4.0</v>
+      </c>
+      <c r="G222" s="20">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="223" ht="15.75" customHeight="1">
+      <c r="A223" s="8">
+        <v>44100.0</v>
+      </c>
+      <c r="B223" s="20">
+        <v>82.0</v>
+      </c>
+      <c r="C223" s="20">
+        <v>3.0</v>
+      </c>
+      <c r="D223" s="20">
+        <v>851.0</v>
+      </c>
+      <c r="E223" s="10">
+        <f t="shared" si="3"/>
+        <v>843</v>
+      </c>
+      <c r="F223" s="20">
+        <v>8.0</v>
+      </c>
+      <c r="G223" s="20">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="224" ht="15.75" customHeight="1">
+      <c r="A224" s="8">
+        <v>44101.0</v>
+      </c>
+      <c r="B224" s="20">
+        <v>150.0</v>
+      </c>
+      <c r="C224" s="20">
+        <v>4.0</v>
+      </c>
+      <c r="D224" s="20">
+        <v>950.0</v>
+      </c>
+      <c r="E224" s="10">
+        <f t="shared" si="3"/>
+        <v>944</v>
+      </c>
+      <c r="F224" s="20">
+        <v>6.0</v>
+      </c>
+      <c r="G224" s="20">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="225" ht="15.75" customHeight="1">
+      <c r="A225" s="8">
+        <v>44102.0</v>
+      </c>
+      <c r="B225" s="21">
+        <v>115.0</v>
+      </c>
+      <c r="C225" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D225" s="21">
+        <v>1011.0</v>
+      </c>
+      <c r="E225" s="10">
+        <f t="shared" si="3"/>
+        <v>1003</v>
+      </c>
+      <c r="F225" s="21">
+        <v>8.0</v>
+      </c>
+      <c r="G225" s="21">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="226" ht="15.75" customHeight="1">
+      <c r="A226" s="8">
+        <v>44103.0</v>
+      </c>
+      <c r="B226" s="21">
+        <v>101.0</v>
+      </c>
+      <c r="C226" s="20">
+        <v>4.0</v>
+      </c>
+      <c r="D226" s="21">
+        <v>1062.0</v>
+      </c>
+      <c r="E226" s="10">
+        <f t="shared" si="3"/>
+        <v>1049</v>
+      </c>
+      <c r="F226" s="21">
+        <v>13.0</v>
+      </c>
+      <c r="G226" s="21">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="227" ht="15.75" customHeight="1">
+      <c r="A227" s="8">
+        <v>44104.0</v>
+      </c>
+      <c r="B227" s="21">
+        <v>89.0</v>
+      </c>
+      <c r="C227" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D227" s="21">
+        <v>1121.0</v>
+      </c>
+      <c r="E227" s="10">
+        <f t="shared" si="3"/>
+        <v>1115</v>
+      </c>
+      <c r="F227" s="20">
+        <v>6.0</v>
+      </c>
+      <c r="G227" s="20">
+        <v>4.0</v>
+      </c>
+    </row>
     <row r="228" ht="15.75" customHeight="1"/>
     <row r="229" ht="15.75" customHeight="1"/>
     <row r="230" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Google mobility, testing and MYS data update.
</commit_message>
<xml_diff>
--- a/data/inputs/covid_mys/COVID_MYS_CASE.xlsx
+++ b/data/inputs/covid_mys/COVID_MYS_CASE.xlsx
@@ -2156,7 +2156,7 @@
         <v>1780.0</v>
       </c>
       <c r="E77" s="10">
-        <f t="shared" ref="E77:E231" si="3">D77-F77</f>
+        <f t="shared" ref="E77:E238" si="3">D77-F77</f>
         <v>1753</v>
       </c>
       <c r="F77" s="19">
@@ -6254,23 +6254,23 @@
       <c r="A228" s="8">
         <v>44105.0</v>
       </c>
-      <c r="B228" s="21">
+      <c r="B228" s="20">
         <v>260.0</v>
       </c>
-      <c r="C228" s="21">
+      <c r="C228" s="20">
         <v>1.0</v>
       </c>
-      <c r="D228" s="21">
+      <c r="D228" s="20">
         <v>1334.0</v>
       </c>
       <c r="E228" s="10">
         <f t="shared" si="3"/>
         <v>1314</v>
       </c>
-      <c r="F228" s="21">
+      <c r="F228" s="20">
         <v>20.0</v>
       </c>
-      <c r="G228" s="21">
+      <c r="G228" s="20">
         <v>3.0</v>
       </c>
     </row>
@@ -6278,23 +6278,23 @@
       <c r="A229" s="8">
         <v>44106.0</v>
       </c>
-      <c r="B229" s="21">
+      <c r="B229" s="20">
         <v>287.0</v>
       </c>
-      <c r="C229" s="21">
+      <c r="C229" s="20">
         <v>0.0</v>
       </c>
-      <c r="D229" s="21">
+      <c r="D229" s="20">
         <v>1540.0</v>
       </c>
       <c r="E229" s="10">
         <f t="shared" si="3"/>
         <v>1518</v>
       </c>
-      <c r="F229" s="21">
+      <c r="F229" s="20">
         <v>22.0</v>
       </c>
-      <c r="G229" s="21">
+      <c r="G229" s="20">
         <v>4.0</v>
       </c>
     </row>
@@ -6302,23 +6302,23 @@
       <c r="A230" s="8">
         <v>44107.0</v>
       </c>
-      <c r="B230" s="21">
+      <c r="B230" s="20">
         <v>317.0</v>
       </c>
-      <c r="C230" s="21">
+      <c r="C230" s="20">
         <v>0.0</v>
       </c>
-      <c r="D230" s="21">
+      <c r="D230" s="20">
         <v>1735.0</v>
       </c>
       <c r="E230" s="10">
         <f t="shared" si="3"/>
         <v>1706</v>
       </c>
-      <c r="F230" s="21">
+      <c r="F230" s="20">
         <v>29.0</v>
       </c>
-      <c r="G230" s="21">
+      <c r="G230" s="20">
         <v>4.0</v>
       </c>
     </row>
@@ -6326,33 +6326,194 @@
       <c r="A231" s="8">
         <v>44108.0</v>
       </c>
-      <c r="B231" s="21">
+      <c r="B231" s="20">
         <v>293.0</v>
       </c>
-      <c r="C231" s="21">
+      <c r="C231" s="20">
         <v>1.0</v>
       </c>
-      <c r="D231" s="21">
+      <c r="D231" s="20">
         <v>1961.0</v>
       </c>
       <c r="E231" s="10">
         <f t="shared" si="3"/>
         <v>1933</v>
       </c>
-      <c r="F231" s="21">
+      <c r="F231" s="20">
         <v>28.0</v>
       </c>
-      <c r="G231" s="21">
+      <c r="G231" s="20">
         <v>4.0</v>
       </c>
     </row>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1">
+      <c r="A232" s="8">
+        <v>44109.0</v>
+      </c>
+      <c r="B232" s="20">
+        <v>432.0</v>
+      </c>
+      <c r="C232" s="20">
+        <v>3.0</v>
+      </c>
+      <c r="D232" s="20">
+        <v>2336.0</v>
+      </c>
+      <c r="E232" s="10">
+        <f t="shared" si="3"/>
+        <v>2304</v>
+      </c>
+      <c r="F232" s="20">
+        <v>32.0</v>
+      </c>
+      <c r="G232" s="20">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="233" ht="15.75" customHeight="1">
+      <c r="A233" s="8">
+        <v>44110.0</v>
+      </c>
+      <c r="B233" s="20">
+        <v>691.0</v>
+      </c>
+      <c r="C233" s="20">
+        <v>3.0</v>
+      </c>
+      <c r="D233" s="20">
+        <v>2936.0</v>
+      </c>
+      <c r="E233" s="10">
+        <f t="shared" si="3"/>
+        <v>2905</v>
+      </c>
+      <c r="F233" s="20">
+        <v>31.0</v>
+      </c>
+      <c r="G233" s="20">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="234" ht="15.75" customHeight="1">
+      <c r="A234" s="8">
+        <v>44111.0</v>
+      </c>
+      <c r="B234" s="20">
+        <v>489.0</v>
+      </c>
+      <c r="C234" s="20">
+        <v>3.0</v>
+      </c>
+      <c r="D234" s="20">
+        <v>3351.0</v>
+      </c>
+      <c r="E234" s="10">
+        <f t="shared" si="3"/>
+        <v>3311</v>
+      </c>
+      <c r="F234" s="20">
+        <v>40.0</v>
+      </c>
+      <c r="G234" s="20">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="235" ht="15.75" customHeight="1">
+      <c r="A235" s="8">
+        <v>44112.0</v>
+      </c>
+      <c r="B235" s="20">
+        <v>375.0</v>
+      </c>
+      <c r="C235" s="20">
+        <v>4.0</v>
+      </c>
+      <c r="D235" s="20">
+        <v>3703.0</v>
+      </c>
+      <c r="E235" s="10">
+        <f t="shared" si="3"/>
+        <v>3643</v>
+      </c>
+      <c r="F235" s="20">
+        <v>60.0</v>
+      </c>
+      <c r="G235" s="20">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="236" ht="15.75" customHeight="1">
+      <c r="A236" s="8">
+        <v>44113.0</v>
+      </c>
+      <c r="B236" s="20">
+        <v>354.0</v>
+      </c>
+      <c r="C236" s="20">
+        <v>2.0</v>
+      </c>
+      <c r="D236" s="20">
+        <v>3863.0</v>
+      </c>
+      <c r="E236" s="10">
+        <f t="shared" si="3"/>
+        <v>3795</v>
+      </c>
+      <c r="F236" s="20">
+        <v>68.0</v>
+      </c>
+      <c r="G236" s="20">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="237" ht="15.75" customHeight="1">
+      <c r="A237" s="8">
+        <v>44114.0</v>
+      </c>
+      <c r="B237" s="20">
+        <v>374.0</v>
+      </c>
+      <c r="C237" s="20">
+        <v>2.0</v>
+      </c>
+      <c r="D237" s="20">
+        <v>4161.0</v>
+      </c>
+      <c r="E237" s="10">
+        <f t="shared" si="3"/>
+        <v>4088</v>
+      </c>
+      <c r="F237" s="20">
+        <v>73.0</v>
+      </c>
+      <c r="G237" s="20">
+        <v>28.0</v>
+      </c>
+    </row>
+    <row r="238" ht="15.75" customHeight="1">
+      <c r="A238" s="8">
+        <v>44115.0</v>
+      </c>
+      <c r="B238" s="21">
+        <v>561.0</v>
+      </c>
+      <c r="C238" s="21">
+        <v>8.0</v>
+      </c>
+      <c r="D238" s="21">
+        <v>4587.0</v>
+      </c>
+      <c r="E238" s="10">
+        <f t="shared" si="3"/>
+        <v>4497</v>
+      </c>
+      <c r="F238" s="21">
+        <v>90.0</v>
+      </c>
+      <c r="G238" s="21">
+        <v>29.0</v>
+      </c>
+    </row>
     <row r="239" ht="15.75" customHeight="1"/>
     <row r="240" ht="15.75" customHeight="1"/>
     <row r="241" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
mys and sabah data import script updated.
</commit_message>
<xml_diff>
--- a/data/inputs/covid_mys/COVID_MYS_CASE.xlsx
+++ b/data/inputs/covid_mys/COVID_MYS_CASE.xlsx
@@ -810,7 +810,7 @@
         <v>2.0</v>
       </c>
       <c r="H24" s="14">
-        <f t="shared" ref="H24:H248" si="2">F24/D24</f>
+        <f t="shared" ref="H24:H252" si="2">F24/D24</f>
         <v>0.0162601626</v>
       </c>
     </row>
@@ -2190,7 +2190,7 @@
         <v>1780.0</v>
       </c>
       <c r="E77" s="12">
-        <f t="shared" ref="E77:E248" si="3">D77-F77</f>
+        <f t="shared" ref="E77:E252" si="3">D77-F77</f>
         <v>1753</v>
       </c>
       <c r="F77" s="21">
@@ -6992,10 +6992,118 @@
         <v>0.01303181296</v>
       </c>
     </row>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1">
+      <c r="A249" s="10">
+        <v>44126.0</v>
+      </c>
+      <c r="B249" s="22">
+        <v>847.0</v>
+      </c>
+      <c r="C249" s="22">
+        <v>5.0</v>
+      </c>
+      <c r="D249" s="22">
+        <v>8183.0</v>
+      </c>
+      <c r="E249" s="12">
+        <f t="shared" si="3"/>
+        <v>8093</v>
+      </c>
+      <c r="F249" s="22">
+        <v>90.0</v>
+      </c>
+      <c r="G249" s="22">
+        <v>29.0</v>
+      </c>
+      <c r="H249" s="14">
+        <f t="shared" si="2"/>
+        <v>0.01099841134</v>
+      </c>
+    </row>
+    <row r="250" ht="15.75" customHeight="1">
+      <c r="A250" s="10">
+        <v>44127.0</v>
+      </c>
+      <c r="B250" s="22">
+        <v>710.0</v>
+      </c>
+      <c r="C250" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="D250" s="22">
+        <v>8416.0</v>
+      </c>
+      <c r="E250" s="12">
+        <f t="shared" si="3"/>
+        <v>8326</v>
+      </c>
+      <c r="F250" s="22">
+        <v>90.0</v>
+      </c>
+      <c r="G250" s="22">
+        <v>28.0</v>
+      </c>
+      <c r="H250" s="14">
+        <f t="shared" si="2"/>
+        <v>0.01069391635</v>
+      </c>
+    </row>
+    <row r="251" ht="15.75" customHeight="1">
+      <c r="A251" s="10">
+        <v>44128.0</v>
+      </c>
+      <c r="B251" s="22">
+        <v>1228.0</v>
+      </c>
+      <c r="C251" s="22">
+        <v>11.0</v>
+      </c>
+      <c r="D251" s="22">
+        <v>8966.0</v>
+      </c>
+      <c r="E251" s="12">
+        <f t="shared" si="3"/>
+        <v>8874</v>
+      </c>
+      <c r="F251" s="22">
+        <v>92.0</v>
+      </c>
+      <c r="G251" s="22">
+        <v>31.0</v>
+      </c>
+      <c r="H251" s="14">
+        <f t="shared" si="2"/>
+        <v>0.01026098595</v>
+      </c>
+    </row>
+    <row r="252" ht="15.75" customHeight="1">
+      <c r="A252" s="10">
+        <v>44129.0</v>
+      </c>
+      <c r="B252" s="22">
+        <v>823.0</v>
+      </c>
+      <c r="C252" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="D252" s="22">
+        <v>9202.0</v>
+      </c>
+      <c r="E252" s="12">
+        <f t="shared" si="3"/>
+        <v>9103</v>
+      </c>
+      <c r="F252" s="22">
+        <v>99.0</v>
+      </c>
+      <c r="G252" s="22">
+        <v>30.0</v>
+      </c>
+      <c r="H252" s="14">
+        <f t="shared" si="2"/>
+        <v>0.01075853075</v>
+      </c>
+    </row>
     <row r="253" ht="15.75" customHeight="1"/>
     <row r="254" ht="15.75" customHeight="1"/>
     <row r="255" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Updates to Malaysia & Sabah
</commit_message>
<xml_diff>
--- a/data/inputs/covid_mys/COVID_MYS_CASE.xlsx
+++ b/data/inputs/covid_mys/COVID_MYS_CASE.xlsx
@@ -810,7 +810,7 @@
         <v>2.0</v>
       </c>
       <c r="H24" s="14">
-        <f t="shared" ref="H24:H252" si="2">F24/D24</f>
+        <f t="shared" ref="H24:H261" si="2">F24/D24</f>
         <v>0.0162601626</v>
       </c>
     </row>
@@ -2190,7 +2190,7 @@
         <v>1780.0</v>
       </c>
       <c r="E77" s="12">
-        <f t="shared" ref="E77:E252" si="3">D77-F77</f>
+        <f t="shared" ref="E77:E261" si="3">D77-F77</f>
         <v>1753</v>
       </c>
       <c r="F77" s="21">
@@ -7104,15 +7104,258 @@
         <v>0.01075853075</v>
       </c>
     </row>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1">
+      <c r="A253" s="10">
+        <v>44130.0</v>
+      </c>
+      <c r="B253" s="22">
+        <v>1240.0</v>
+      </c>
+      <c r="C253" s="22">
+        <v>2.0</v>
+      </c>
+      <c r="D253" s="22">
+        <v>9744.0</v>
+      </c>
+      <c r="E253" s="12">
+        <f t="shared" si="3"/>
+        <v>9650</v>
+      </c>
+      <c r="F253" s="22">
+        <v>94.0</v>
+      </c>
+      <c r="G253" s="22">
+        <v>31.0</v>
+      </c>
+      <c r="H253" s="14">
+        <f t="shared" si="2"/>
+        <v>0.009646962233</v>
+      </c>
+    </row>
+    <row r="254" ht="15.75" customHeight="1">
+      <c r="A254" s="10">
+        <v>44131.0</v>
+      </c>
+      <c r="B254" s="22">
+        <v>835.0</v>
+      </c>
+      <c r="C254" s="22">
+        <v>5.0</v>
+      </c>
+      <c r="D254" s="22">
+        <v>9903.0</v>
+      </c>
+      <c r="E254" s="12">
+        <f t="shared" si="3"/>
+        <v>9814</v>
+      </c>
+      <c r="F254" s="22">
+        <v>89.0</v>
+      </c>
+      <c r="G254" s="22">
+        <v>32.0</v>
+      </c>
+      <c r="H254" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008987175603</v>
+      </c>
+    </row>
+    <row r="255" ht="15.75" customHeight="1">
+      <c r="A255" s="10">
+        <v>44132.0</v>
+      </c>
+      <c r="B255" s="22">
+        <v>801.0</v>
+      </c>
+      <c r="C255" s="22">
+        <v>2.0</v>
+      </c>
+      <c r="D255" s="22">
+        <v>10123.0</v>
+      </c>
+      <c r="E255" s="12">
+        <f t="shared" si="3"/>
+        <v>10029</v>
+      </c>
+      <c r="F255" s="22">
+        <v>94.0</v>
+      </c>
+      <c r="G255" s="22">
+        <v>25.0</v>
+      </c>
+      <c r="H255" s="14">
+        <f t="shared" si="2"/>
+        <v>0.009285784846</v>
+      </c>
+    </row>
+    <row r="256" ht="15.75" customHeight="1">
+      <c r="A256" s="10">
+        <v>44133.0</v>
+      </c>
+      <c r="B256" s="22">
+        <v>649.0</v>
+      </c>
+      <c r="C256" s="22">
+        <v>7.0</v>
+      </c>
+      <c r="D256" s="22">
+        <v>10087.0</v>
+      </c>
+      <c r="E256" s="12">
+        <f t="shared" si="3"/>
+        <v>9981</v>
+      </c>
+      <c r="F256" s="22">
+        <v>106.0</v>
+      </c>
+      <c r="G256" s="22">
+        <v>23.0</v>
+      </c>
+      <c r="H256" s="14">
+        <f t="shared" si="2"/>
+        <v>0.01050857539</v>
+      </c>
+    </row>
+    <row r="257" ht="15.75" customHeight="1">
+      <c r="A257" s="10">
+        <v>44134.0</v>
+      </c>
+      <c r="B257" s="22">
+        <v>799.0</v>
+      </c>
+      <c r="C257" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="D257" s="22">
+        <v>10392.0</v>
+      </c>
+      <c r="E257" s="12">
+        <f t="shared" si="3"/>
+        <v>10302</v>
+      </c>
+      <c r="F257" s="22">
+        <v>90.0</v>
+      </c>
+      <c r="G257" s="22">
+        <v>20.0</v>
+      </c>
+      <c r="H257" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008660508083</v>
+      </c>
+    </row>
+    <row r="258" ht="15.75" customHeight="1">
+      <c r="A258" s="10">
+        <v>44135.0</v>
+      </c>
+      <c r="B258" s="22">
+        <v>659.0</v>
+      </c>
+      <c r="C258" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="D258" s="22">
+        <v>10051.0</v>
+      </c>
+      <c r="E258" s="12">
+        <f t="shared" si="3"/>
+        <v>9968</v>
+      </c>
+      <c r="F258" s="22">
+        <v>83.0</v>
+      </c>
+      <c r="G258" s="22">
+        <v>19.0</v>
+      </c>
+      <c r="H258" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008257884788</v>
+      </c>
+    </row>
+    <row r="259" ht="15.75" customHeight="1">
+      <c r="A259" s="10">
+        <v>44136.0</v>
+      </c>
+      <c r="B259" s="22">
+        <v>957.0</v>
+      </c>
+      <c r="C259" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="D259" s="22">
+        <v>10036.0</v>
+      </c>
+      <c r="E259" s="12">
+        <f t="shared" si="3"/>
+        <v>9939</v>
+      </c>
+      <c r="F259" s="22">
+        <v>97.0</v>
+      </c>
+      <c r="G259" s="22">
+        <v>27.0</v>
+      </c>
+      <c r="H259" s="14">
+        <f t="shared" si="2"/>
+        <v>0.009665205261</v>
+      </c>
+    </row>
+    <row r="260" ht="15.75" customHeight="1">
+      <c r="A260" s="10">
+        <v>44137.0</v>
+      </c>
+      <c r="B260" s="22">
+        <v>834.0</v>
+      </c>
+      <c r="C260" s="22">
+        <v>3.0</v>
+      </c>
+      <c r="D260" s="22">
+        <v>9968.0</v>
+      </c>
+      <c r="E260" s="12">
+        <f t="shared" si="3"/>
+        <v>9877</v>
+      </c>
+      <c r="F260" s="22">
+        <v>91.0</v>
+      </c>
+      <c r="G260" s="22">
+        <v>32.0</v>
+      </c>
+      <c r="H260" s="14">
+        <f t="shared" si="2"/>
+        <v>0.009129213483</v>
+      </c>
+    </row>
+    <row r="261" ht="15.75" customHeight="1">
+      <c r="A261" s="10">
+        <v>44138.0</v>
+      </c>
+      <c r="B261" s="22">
+        <v>1054.0</v>
+      </c>
+      <c r="C261" s="22">
+        <v>14.0</v>
+      </c>
+      <c r="D261" s="22">
+        <v>10135.0</v>
+      </c>
+      <c r="E261" s="12">
+        <f t="shared" si="3"/>
+        <v>10041</v>
+      </c>
+      <c r="F261" s="22">
+        <v>94.0</v>
+      </c>
+      <c r="G261" s="22">
+        <v>32.0</v>
+      </c>
+      <c r="H261" s="14">
+        <f t="shared" si="2"/>
+        <v>0.009274790331</v>
+      </c>
+    </row>
     <row r="262" ht="15.75" customHeight="1"/>
     <row r="263" ht="15.75" customHeight="1"/>
     <row r="264" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Google mobility and MYS update
</commit_message>
<xml_diff>
--- a/data/inputs/covid_mys/COVID_MYS_CASE.xlsx
+++ b/data/inputs/covid_mys/COVID_MYS_CASE.xlsx
@@ -73,7 +73,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\ mmm"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -95,6 +95,11 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -160,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -225,6 +230,12 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="16" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -810,7 +821,7 @@
         <v>2.0</v>
       </c>
       <c r="H24" s="14">
-        <f t="shared" ref="H24:H261" si="2">F24/D24</f>
+        <f t="shared" ref="H24:H267" si="2">F24/D24</f>
         <v>0.0162601626</v>
       </c>
     </row>
@@ -2190,7 +2201,7 @@
         <v>1780.0</v>
       </c>
       <c r="E77" s="12">
-        <f t="shared" ref="E77:E261" si="3">D77-F77</f>
+        <f t="shared" ref="E77:E267" si="3">D77-F77</f>
         <v>1753</v>
       </c>
       <c r="F77" s="21">
@@ -7356,12 +7367,174 @@
         <v>0.009274790331</v>
       </c>
     </row>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1">
+      <c r="A262" s="10">
+        <v>44139.0</v>
+      </c>
+      <c r="B262" s="23">
+        <v>1032.0</v>
+      </c>
+      <c r="C262" s="23">
+        <v>3.0</v>
+      </c>
+      <c r="D262" s="23">
+        <v>10339.0</v>
+      </c>
+      <c r="E262" s="12">
+        <f t="shared" si="3"/>
+        <v>10257</v>
+      </c>
+      <c r="F262" s="23">
+        <v>82.0</v>
+      </c>
+      <c r="G262" s="23">
+        <v>27.0</v>
+      </c>
+      <c r="H262" s="14">
+        <f t="shared" si="2"/>
+        <v>0.007931134539</v>
+      </c>
+    </row>
+    <row r="263" ht="15.75" customHeight="1">
+      <c r="A263" s="10">
+        <v>44140.0</v>
+      </c>
+      <c r="B263" s="23">
+        <v>1009.0</v>
+      </c>
+      <c r="C263" s="23">
+        <v>9.0</v>
+      </c>
+      <c r="D263" s="23">
+        <v>10503.0</v>
+      </c>
+      <c r="E263" s="12">
+        <f t="shared" si="3"/>
+        <v>10425</v>
+      </c>
+      <c r="F263" s="23">
+        <v>78.0</v>
+      </c>
+      <c r="G263" s="23">
+        <v>28.0</v>
+      </c>
+      <c r="H263" s="14">
+        <f t="shared" si="2"/>
+        <v>0.007426449586</v>
+      </c>
+    </row>
+    <row r="264" ht="15.75" customHeight="1">
+      <c r="A264" s="10">
+        <v>44141.0</v>
+      </c>
+      <c r="B264" s="23">
+        <v>1755.0</v>
+      </c>
+      <c r="C264" s="23">
+        <v>3.0</v>
+      </c>
+      <c r="D264" s="23">
+        <v>11530.0</v>
+      </c>
+      <c r="E264" s="12">
+        <f t="shared" si="3"/>
+        <v>11447</v>
+      </c>
+      <c r="F264" s="23">
+        <v>83.0</v>
+      </c>
+      <c r="G264" s="23">
+        <v>32.0</v>
+      </c>
+      <c r="H264" s="14">
+        <f t="shared" si="2"/>
+        <v>0.007198612316</v>
+      </c>
+    </row>
+    <row r="265" ht="15.75" customHeight="1">
+      <c r="A265" s="10">
+        <v>44142.0</v>
+      </c>
+      <c r="B265" s="23">
+        <v>1168.0</v>
+      </c>
+      <c r="C265" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="D265" s="23">
+        <v>11666.0</v>
+      </c>
+      <c r="E265" s="12">
+        <f t="shared" si="3"/>
+        <v>11579</v>
+      </c>
+      <c r="F265" s="23">
+        <v>87.0</v>
+      </c>
+      <c r="G265" s="23">
+        <v>32.0</v>
+      </c>
+      <c r="H265" s="14">
+        <f t="shared" si="2"/>
+        <v>0.007457569004</v>
+      </c>
+    </row>
+    <row r="266" ht="15.75" customHeight="1">
+      <c r="A266" s="10">
+        <v>44143.0</v>
+      </c>
+      <c r="B266" s="23">
+        <v>852.0</v>
+      </c>
+      <c r="C266" s="23">
+        <v>13.0</v>
+      </c>
+      <c r="D266" s="23">
+        <v>11689.0</v>
+      </c>
+      <c r="E266" s="12">
+        <f t="shared" si="3"/>
+        <v>11595</v>
+      </c>
+      <c r="F266" s="23">
+        <v>94.0</v>
+      </c>
+      <c r="G266" s="23">
+        <v>32.0</v>
+      </c>
+      <c r="H266" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008041748653</v>
+      </c>
+    </row>
+    <row r="267" ht="15.75" customHeight="1">
+      <c r="A267" s="24">
+        <v>44144.0</v>
+      </c>
+      <c r="B267" s="22">
+        <v>972.0</v>
+      </c>
+      <c r="C267" s="22">
+        <v>5.0</v>
+      </c>
+      <c r="D267" s="22">
+        <v>11308.0</v>
+      </c>
+      <c r="E267" s="12">
+        <f t="shared" si="3"/>
+        <v>11222</v>
+      </c>
+      <c r="F267" s="22">
+        <v>86.0</v>
+      </c>
+      <c r="G267" s="22">
+        <v>31.0</v>
+      </c>
+      <c r="H267" s="14">
+        <f t="shared" si="2"/>
+        <v>0.007605235232</v>
+      </c>
+    </row>
     <row r="268" ht="15.75" customHeight="1"/>
     <row r="269" ht="15.75" customHeight="1"/>
     <row r="270" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Mobility, testing and MYS data update
</commit_message>
<xml_diff>
--- a/data/inputs/covid_mys/COVID_MYS_CASE.xlsx
+++ b/data/inputs/covid_mys/COVID_MYS_CASE.xlsx
@@ -234,8 +234,8 @@
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="16" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -821,7 +821,7 @@
         <v>2.0</v>
       </c>
       <c r="H24" s="14">
-        <f t="shared" ref="H24:H267" si="2">F24/D24</f>
+        <f t="shared" ref="H24:H287" si="2">F24/D24</f>
         <v>0.0162601626</v>
       </c>
     </row>
@@ -2201,7 +2201,7 @@
         <v>1780.0</v>
       </c>
       <c r="E77" s="12">
-        <f t="shared" ref="E77:E267" si="3">D77-F77</f>
+        <f t="shared" ref="E77:E287" si="3">D77-F77</f>
         <v>1753</v>
       </c>
       <c r="F77" s="21">
@@ -7508,7 +7508,7 @@
       </c>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="A267" s="24">
+      <c r="A267" s="10">
         <v>44144.0</v>
       </c>
       <c r="B267" s="22">
@@ -7535,26 +7535,566 @@
         <v>0.007605235232</v>
       </c>
     </row>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1">
+      <c r="A268" s="10">
+        <v>44145.0</v>
+      </c>
+      <c r="B268" s="22">
+        <v>869.0</v>
+      </c>
+      <c r="C268" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="D268" s="22">
+        <v>11446.0</v>
+      </c>
+      <c r="E268" s="12">
+        <f t="shared" si="3"/>
+        <v>11364</v>
+      </c>
+      <c r="F268" s="22">
+        <v>82.0</v>
+      </c>
+      <c r="G268" s="22">
+        <v>27.0</v>
+      </c>
+      <c r="H268" s="14">
+        <f t="shared" si="2"/>
+        <v>0.007164074786</v>
+      </c>
+    </row>
+    <row r="269" ht="15.75" customHeight="1">
+      <c r="A269" s="10">
+        <v>44146.0</v>
+      </c>
+      <c r="B269" s="22">
+        <v>822.0</v>
+      </c>
+      <c r="C269" s="22">
+        <v>7.0</v>
+      </c>
+      <c r="D269" s="22">
+        <v>11497.0</v>
+      </c>
+      <c r="E269" s="12">
+        <f t="shared" si="3"/>
+        <v>11411</v>
+      </c>
+      <c r="F269" s="22">
+        <v>86.0</v>
+      </c>
+      <c r="G269" s="22">
+        <v>30.0</v>
+      </c>
+      <c r="H269" s="14">
+        <f t="shared" si="2"/>
+        <v>0.007480212229</v>
+      </c>
+    </row>
+    <row r="270" ht="15.75" customHeight="1">
+      <c r="A270" s="10">
+        <v>44147.0</v>
+      </c>
+      <c r="B270" s="22">
+        <v>919.0</v>
+      </c>
+      <c r="C270" s="22">
+        <v>3.0</v>
+      </c>
+      <c r="D270" s="22">
+        <v>11419.0</v>
+      </c>
+      <c r="E270" s="12">
+        <f t="shared" si="3"/>
+        <v>11327</v>
+      </c>
+      <c r="F270" s="22">
+        <v>92.0</v>
+      </c>
+      <c r="G270" s="22">
+        <v>35.0</v>
+      </c>
+      <c r="H270" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008056747526</v>
+      </c>
+    </row>
+    <row r="271" ht="15.75" customHeight="1">
+      <c r="A271" s="10">
+        <v>44148.0</v>
+      </c>
+      <c r="B271" s="22">
+        <v>1304.0</v>
+      </c>
+      <c r="C271" s="22">
+        <v>4.0</v>
+      </c>
+      <c r="D271" s="22">
+        <v>11822.0</v>
+      </c>
+      <c r="E271" s="12">
+        <f t="shared" si="3"/>
+        <v>11726</v>
+      </c>
+      <c r="F271" s="22">
+        <v>96.0</v>
+      </c>
+      <c r="G271" s="22">
+        <v>39.0</v>
+      </c>
+      <c r="H271" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008120453392</v>
+      </c>
+    </row>
+    <row r="272" ht="15.75" customHeight="1">
+      <c r="A272" s="10">
+        <v>44149.0</v>
+      </c>
+      <c r="B272" s="22">
+        <v>1114.0</v>
+      </c>
+      <c r="C272" s="22">
+        <v>2.0</v>
+      </c>
+      <c r="D272" s="22">
+        <v>12131.0</v>
+      </c>
+      <c r="E272" s="12">
+        <f t="shared" si="3"/>
+        <v>12028</v>
+      </c>
+      <c r="F272" s="22">
+        <v>103.0</v>
+      </c>
+      <c r="G272" s="22">
+        <v>43.0</v>
+      </c>
+      <c r="H272" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008490643805</v>
+      </c>
+    </row>
+    <row r="273" ht="15.75" customHeight="1">
+      <c r="A273" s="10">
+        <v>44150.0</v>
+      </c>
+      <c r="B273" s="22">
+        <v>1208.0</v>
+      </c>
+      <c r="C273" s="22">
+        <v>6.0</v>
+      </c>
+      <c r="D273" s="22">
+        <v>12323.0</v>
+      </c>
+      <c r="E273" s="12">
+        <f t="shared" si="3"/>
+        <v>12219</v>
+      </c>
+      <c r="F273" s="22">
+        <v>104.0</v>
+      </c>
+      <c r="G273" s="22">
+        <v>42.0</v>
+      </c>
+      <c r="H273" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008439503368</v>
+      </c>
+    </row>
+    <row r="274" ht="15.75" customHeight="1">
+      <c r="A274" s="10">
+        <v>44151.0</v>
+      </c>
+      <c r="B274" s="22">
+        <v>1103.0</v>
+      </c>
+      <c r="C274" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="D274" s="22">
+        <v>12601.0</v>
+      </c>
+      <c r="E274" s="12">
+        <f t="shared" si="3"/>
+        <v>12499</v>
+      </c>
+      <c r="F274" s="22">
+        <v>102.0</v>
+      </c>
+      <c r="G274" s="22">
+        <v>39.0</v>
+      </c>
+      <c r="H274" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008094595667</v>
+      </c>
+    </row>
+    <row r="275" ht="15.75" customHeight="1">
+      <c r="A275" s="10">
+        <v>44152.0</v>
+      </c>
+      <c r="B275" s="22">
+        <v>1210.0</v>
+      </c>
+      <c r="C275" s="22">
+        <v>19.0</v>
+      </c>
+      <c r="D275" s="22">
+        <v>12788.0</v>
+      </c>
+      <c r="E275" s="12">
+        <f t="shared" si="3"/>
+        <v>12683</v>
+      </c>
+      <c r="F275" s="22">
+        <v>105.0</v>
+      </c>
+      <c r="G275" s="22">
+        <v>40.0</v>
+      </c>
+      <c r="H275" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008210822646</v>
+      </c>
+    </row>
+    <row r="276" ht="15.75" customHeight="1">
+      <c r="A276" s="10">
+        <v>44153.0</v>
+      </c>
+      <c r="B276" s="22">
+        <v>660.0</v>
+      </c>
+      <c r="C276" s="22">
+        <v>4.0</v>
+      </c>
+      <c r="D276" s="22">
+        <v>12814.0</v>
+      </c>
+      <c r="E276" s="12">
+        <f t="shared" si="3"/>
+        <v>12711</v>
+      </c>
+      <c r="F276" s="22">
+        <v>103.0</v>
+      </c>
+      <c r="G276" s="22">
+        <v>41.0</v>
+      </c>
+      <c r="H276" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008038083346</v>
+      </c>
+    </row>
+    <row r="277" ht="15.75" customHeight="1">
+      <c r="A277" s="10">
+        <v>44154.0</v>
+      </c>
+      <c r="B277" s="22">
+        <v>1290.0</v>
+      </c>
+      <c r="C277" s="22">
+        <v>5.0</v>
+      </c>
+      <c r="D277" s="22">
+        <v>13222.0</v>
+      </c>
+      <c r="E277" s="12">
+        <f t="shared" si="3"/>
+        <v>13112</v>
+      </c>
+      <c r="F277" s="22">
+        <v>110.0</v>
+      </c>
+      <c r="G277" s="22">
+        <v>37.0</v>
+      </c>
+      <c r="H277" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008319467554</v>
+      </c>
+    </row>
+    <row r="278" ht="15.75" customHeight="1">
+      <c r="A278" s="10">
+        <v>44155.0</v>
+      </c>
+      <c r="B278" s="22">
+        <v>958.0</v>
+      </c>
+      <c r="C278" s="22">
+        <v>5.0</v>
+      </c>
+      <c r="D278" s="22">
+        <v>13221.0</v>
+      </c>
+      <c r="E278" s="12">
+        <f t="shared" si="3"/>
+        <v>13111</v>
+      </c>
+      <c r="F278" s="22">
+        <v>110.0</v>
+      </c>
+      <c r="G278" s="22">
+        <v>42.0</v>
+      </c>
+      <c r="H278" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008320096816</v>
+      </c>
+    </row>
+    <row r="279" ht="15.75" customHeight="1">
+      <c r="A279" s="10">
+        <v>44156.0</v>
+      </c>
+      <c r="B279" s="22">
+        <v>1041.0</v>
+      </c>
+      <c r="C279" s="22">
+        <v>2.0</v>
+      </c>
+      <c r="D279" s="22">
+        <v>12854.0</v>
+      </c>
+      <c r="E279" s="12">
+        <f t="shared" si="3"/>
+        <v>12746</v>
+      </c>
+      <c r="F279" s="22">
+        <v>108.0</v>
+      </c>
+      <c r="G279" s="22">
+        <v>45.0</v>
+      </c>
+      <c r="H279" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008402053835</v>
+      </c>
+    </row>
+    <row r="280" ht="15.75" customHeight="1">
+      <c r="A280" s="10">
+        <v>44157.0</v>
+      </c>
+      <c r="B280" s="22">
+        <v>1096.0</v>
+      </c>
+      <c r="C280" s="22">
+        <v>6.0</v>
+      </c>
+      <c r="D280" s="22">
+        <v>12843.0</v>
+      </c>
+      <c r="E280" s="12">
+        <f t="shared" si="3"/>
+        <v>12737</v>
+      </c>
+      <c r="F280" s="22">
+        <v>106.0</v>
+      </c>
+      <c r="G280" s="22">
+        <v>46.0</v>
+      </c>
+      <c r="H280" s="14">
+        <f t="shared" si="2"/>
+        <v>0.00825352332</v>
+      </c>
+    </row>
+    <row r="281" ht="15.75" customHeight="1">
+      <c r="A281" s="10">
+        <v>44158.0</v>
+      </c>
+      <c r="B281" s="22">
+        <v>1884.0</v>
+      </c>
+      <c r="C281" s="22">
+        <v>2.0</v>
+      </c>
+      <c r="D281" s="22">
+        <v>13842.0</v>
+      </c>
+      <c r="E281" s="12">
+        <f t="shared" si="3"/>
+        <v>13727</v>
+      </c>
+      <c r="F281" s="22">
+        <v>115.0</v>
+      </c>
+      <c r="G281" s="22">
+        <v>48.0</v>
+      </c>
+      <c r="H281" s="14">
+        <f t="shared" si="2"/>
+        <v>0.00830804797</v>
+      </c>
+    </row>
+    <row r="282" ht="15.75" customHeight="1">
+      <c r="A282" s="10">
+        <v>44159.0</v>
+      </c>
+      <c r="B282" s="22">
+        <v>2188.0</v>
+      </c>
+      <c r="C282" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="D282" s="22">
+        <v>14353.0</v>
+      </c>
+      <c r="E282" s="12">
+        <f t="shared" si="3"/>
+        <v>14241</v>
+      </c>
+      <c r="F282" s="22">
+        <v>112.0</v>
+      </c>
+      <c r="G282" s="22">
+        <v>49.0</v>
+      </c>
+      <c r="H282" s="14">
+        <f t="shared" si="2"/>
+        <v>0.007803246708</v>
+      </c>
+    </row>
+    <row r="283" ht="15.75" customHeight="1">
+      <c r="A283" s="10">
+        <v>44160.0</v>
+      </c>
+      <c r="B283" s="24">
+        <v>970.0</v>
+      </c>
+      <c r="C283" s="24">
+        <v>5.0</v>
+      </c>
+      <c r="D283" s="24">
+        <v>12971.0</v>
+      </c>
+      <c r="E283" s="12">
+        <f t="shared" si="3"/>
+        <v>12861</v>
+      </c>
+      <c r="F283" s="24">
+        <v>110.0</v>
+      </c>
+      <c r="G283" s="24">
+        <v>47.0</v>
+      </c>
+      <c r="H283" s="14">
+        <f t="shared" si="2"/>
+        <v>0.008480456403</v>
+      </c>
+    </row>
+    <row r="284" ht="15.75" customHeight="1">
+      <c r="A284" s="10">
+        <v>44161.0</v>
+      </c>
+      <c r="B284" s="24">
+        <v>935.0</v>
+      </c>
+      <c r="C284" s="24">
+        <v>4.0</v>
+      </c>
+      <c r="D284" s="24">
+        <v>11348.0</v>
+      </c>
+      <c r="E284" s="12">
+        <f t="shared" si="3"/>
+        <v>11238</v>
+      </c>
+      <c r="F284" s="24">
+        <v>110.0</v>
+      </c>
+      <c r="G284" s="24">
+        <v>45.0</v>
+      </c>
+      <c r="H284" s="14">
+        <f t="shared" si="2"/>
+        <v>0.009693338033</v>
+      </c>
+    </row>
+    <row r="285" ht="15.75" customHeight="1">
+      <c r="A285" s="10">
+        <v>44162.0</v>
+      </c>
+      <c r="B285" s="24">
+        <v>1109.0</v>
+      </c>
+      <c r="C285" s="24">
+        <v>10.0</v>
+      </c>
+      <c r="D285" s="24">
+        <v>11307.0</v>
+      </c>
+      <c r="E285" s="12">
+        <f t="shared" si="3"/>
+        <v>11194</v>
+      </c>
+      <c r="F285" s="24">
+        <v>113.0</v>
+      </c>
+      <c r="G285" s="24">
+        <v>41.0</v>
+      </c>
+      <c r="H285" s="14">
+        <f t="shared" si="2"/>
+        <v>0.009993809145</v>
+      </c>
+    </row>
+    <row r="286" ht="15.75" customHeight="1">
+      <c r="A286" s="10">
+        <v>44163.0</v>
+      </c>
+      <c r="B286" s="24">
+        <v>1315.0</v>
+      </c>
+      <c r="C286" s="24">
+        <v>5.0</v>
+      </c>
+      <c r="D286" s="24">
+        <v>11508.0</v>
+      </c>
+      <c r="E286" s="12">
+        <f t="shared" si="3"/>
+        <v>11390</v>
+      </c>
+      <c r="F286" s="24">
+        <v>118.0</v>
+      </c>
+      <c r="G286" s="24">
+        <v>43.0</v>
+      </c>
+      <c r="H286" s="14">
+        <f t="shared" si="2"/>
+        <v>0.01025373653</v>
+      </c>
+    </row>
+    <row r="287" ht="15.75" customHeight="1">
+      <c r="A287" s="10">
+        <v>44164.0</v>
+      </c>
+      <c r="B287" s="24">
+        <v>1309.0</v>
+      </c>
+      <c r="C287" s="24">
+        <v>1.0</v>
+      </c>
+      <c r="D287" s="24">
+        <v>11481.0</v>
+      </c>
+      <c r="E287" s="12">
+        <f t="shared" si="3"/>
+        <v>11365</v>
+      </c>
+      <c r="F287" s="24">
+        <v>116.0</v>
+      </c>
+      <c r="G287" s="24">
+        <v>42.0</v>
+      </c>
+      <c r="H287" s="14">
+        <f t="shared" si="2"/>
+        <v>0.01010364951</v>
+      </c>
+    </row>
     <row r="288" ht="15.75" customHeight="1"/>
     <row r="289" ht="15.75" customHeight="1"/>
     <row r="290" ht="15.75" customHeight="1"/>

</xml_diff>